<commit_message>
hall effect and capactive datasets recorded
</commit_message>
<xml_diff>
--- a/FingertipList.xlsx
+++ b/FingertipList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/dsh46_cam_ac_uk/Documents/Documents/EPFL/Fingertips/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{175CE505-BF2F-4DED-BA62-73C609B74BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD459763-7DEB-4E19-8B57-54A5DF561E6C}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{175CE505-BF2F-4DED-BA62-73C609B74BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4077B64-7A2D-4226-919F-BD652D120060}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="22116" windowHeight="9960" xr2:uid="{D43F7A13-62A2-4422-9A8B-F7EF72E31FFA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D43F7A13-62A2-4422-9A8B-F7EF72E31FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>T2</t>
-  </si>
-  <si>
-    <t>Sudong?</t>
   </si>
   <si>
     <t>Also expect second versions of some of these</t>
@@ -168,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,16 +181,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,12 +192,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,13 +208,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +598,7 @@
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -783,10 +763,10 @@
       <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="3"/>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -798,7 +778,7 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="2"/>
@@ -835,7 +815,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -847,13 +827,13 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final experiments completed with double setup
</commit_message>
<xml_diff>
--- a/FingertipList.xlsx
+++ b/FingertipList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/dsh46_cam_ac_uk/Documents/Documents/EPFL/Fingertips/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{175CE505-BF2F-4DED-BA62-73C609B74BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4077B64-7A2D-4226-919F-BD652D120060}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{175CE505-BF2F-4DED-BA62-73C609B74BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D71C27BE-35EA-4683-AB1D-D3BA60042B86}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D43F7A13-62A2-4422-9A8B-F7EF72E31FFA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{D43F7A13-62A2-4422-9A8B-F7EF72E31FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>Hall effect</t>
   </si>
   <si>
-    <t>Capacitive?</t>
-  </si>
-  <si>
     <t>Solid silicone (passive)</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>F2</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Anisotropic TPU B (passive)</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Capacitive</t>
   </si>
 </sst>
 </file>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C018DC3C-0E05-48B7-B7DA-6FB44C5E73F4}">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -641,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -656,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -671,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -686,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -713,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -743,7 +743,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -758,7 +758,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -773,10 +773,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
@@ -788,10 +788,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -800,10 +800,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -812,10 +812,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -824,16 +824,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>